<commit_message>
Add pagination to Mapped TB and TB2 tables with page size controls and fix Edit/Delete button layout wrapping
</commit_message>
<xml_diff>
--- a/SRM_Pro/TB format.xlsx
+++ b/SRM_Pro/TB format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ICAI_Audit_Tool\nw\SRM_Pro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393DCD67-765C-4CF5-ABC8-FF127A29585F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FCEFA9-27F7-40FF-92A9-F8EDD806E4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{024B333F-E51D-4051-BE86-FFC39602633C}"/>
   </bookViews>
@@ -1293,7 +1293,7 @@
   <dimension ref="A1:U198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>